<commit_message>
Finished implimenting solve_sudoku, results are not great.
</commit_message>
<xml_diff>
--- a/notes/grid_indexing.xlsx
+++ b/notes/grid_indexing.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7635" xr2:uid="{E5CC09FB-E5CC-47FD-BE8B-B78BB9842D2D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Indexing" sheetId="1" r:id="rId1"/>
+    <sheet name="Grid1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -35,7 +36,7 @@
     <t>int(i/9/3)</t>
   </si>
   <si>
-    <t>(I % 9 % 3)</t>
+    <t>(I % 9 / 3)</t>
   </si>
 </sst>
 </file>
@@ -59,7 +60,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -147,11 +148,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -163,6 +201,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,4 +906,280 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C7E786-090A-4214-940E-77FE0995D3FF}">
+  <dimension ref="B2:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5">
+        <v>3</v>
+      </c>
+      <c r="H3" s="4">
+        <v>8</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4">
+        <v>4</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>4</v>
+      </c>
+      <c r="J5" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>8</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>9</v>
+      </c>
+      <c r="I6" s="5">
+        <v>5</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7">
+        <v>4</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8">
+        <v>5</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>7</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>6</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>8</v>
+      </c>
+      <c r="J9" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>8</v>
+      </c>
+      <c r="D10" s="8">
+        <v>6</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>7</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>2</v>
+      </c>
+      <c r="J10" s="9">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Got a working solution in solve_sudoku_clean.py
</commit_message>
<xml_diff>
--- a/notes/grid_indexing.xlsx
+++ b/notes/grid_indexing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7635" xr2:uid="{E5CC09FB-E5CC-47FD-BE8B-B78BB9842D2D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="1" xr2:uid="{E5CC09FB-E5CC-47FD-BE8B-B78BB9842D2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Indexing" sheetId="1" r:id="rId1"/>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27ED68BC-11C1-40E0-BC3A-D10EEF68A86E}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -912,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C7E786-090A-4214-940E-77FE0995D3FF}">
   <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>